<commit_message>
Fix Country/Region and collect.py file
</commit_message>
<xml_diff>
--- a/Challenge3/Duplicate Contact Records Found by Phone Number.xlsx
+++ b/Challenge3/Duplicate Contact Records Found by Phone Number.xlsx
@@ -477,10 +477,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2459</v>
+        <v>6772</v>
       </c>
       <c r="B2" t="n">
-        <v>132924337805</v>
+        <v>134659261811</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -500,12 +500,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Balham   Vale, 5116</t>
+          <t>Eldon  Lane, 7122</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924337805</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134659261811</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -516,10 +516,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>317</v>
+        <v>2023</v>
       </c>
       <c r="B3" t="n">
-        <v>132924473401</v>
+        <v>134628036652</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -531,11 +531,7 @@
           <t>Newman</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>tyson_newman1021718471+103@yahoo.com</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)6835 027381</t>
@@ -543,12 +539,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Apollo  Crossroad, 6027</t>
+          <t>Balham   Vale, 5116</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924473401</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134628036652</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -559,10 +555,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>6607</v>
+        <v>387</v>
       </c>
       <c r="B4" t="n">
-        <v>132915056185</v>
+        <v>134626306081</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -574,7 +570,11 @@
           <t>Newman</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>tyson_newman1021718471+103@yahoo.com</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)6835 027381</t>
@@ -582,12 +582,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Eldon  Lane, 7122</t>
+          <t>Apollo  Crossroad, 6027</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915056185</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626306081</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -598,10 +598,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>561</v>
+        <v>488</v>
       </c>
       <c r="B5" t="n">
-        <v>132916656022</v>
+        <v>134630045254</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -615,7 +615,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>sebastian_parker1458479109+102@joiniaa.com</t>
+          <t>sebastian_parker1458479109@joiniaa.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -625,12 +625,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Arbutus   Crossroad, 4836</t>
+          <t>Bales  Grove, 8324</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916656022</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630045254</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -641,10 +641,10 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>286</v>
+        <v>654</v>
       </c>
       <c r="B6" t="n">
-        <v>132911795531</v>
+        <v>134660841279</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -658,7 +658,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>sebastian_parker1458479109@joiniaa.com</t>
+          <t>sebastian_parker1458479109+102@joiniaa.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -668,12 +668,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Bales  Grove, 8324</t>
+          <t>Arbutus   Crossroad, 4836</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911795531</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660841279</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -684,10 +684,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>559</v>
+        <v>646</v>
       </c>
       <c r="B7" t="n">
-        <v>132914154500</v>
+        <v>134626787677</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914154500</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626787677</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -727,10 +727,10 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>5567</v>
+        <v>1151</v>
       </c>
       <c r="B8" t="n">
-        <v>132911795469</v>
+        <v>134631191657</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -742,7 +742,11 @@
           <t>Welsch</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ryan_welsch107397896+104@famism.biz</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)2778 635604</t>
@@ -750,12 +754,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Monroe Alley, 2353</t>
+          <t>Collingwood  Road, 454</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911795469</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134631191657</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -766,10 +770,10 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>140</v>
+        <v>2977</v>
       </c>
       <c r="B9" t="n">
-        <v>132912623361</v>
+        <v>134654791766</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -781,11 +785,7 @@
           <t>Welsch</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ryan_welsch107397896+103@famism.biz</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)2778 635604</t>
@@ -793,12 +793,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Thorndike   Walk, 1902</t>
+          <t>Monroe Alley, 2353</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912623361</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134654791766</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -809,10 +809,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>618</v>
+        <v>276</v>
       </c>
       <c r="B10" t="n">
-        <v>132919827222</v>
+        <v>134625997060</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -826,7 +826,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ryan_welsch107397896+104@famism.biz</t>
+          <t>ryan_welsch107397896+103@famism.biz</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Collingwood  Road, 454</t>
+          <t>Thorndike   Walk, 1902</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919827222</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134625997060</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -852,10 +852,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>5014</v>
+        <v>4040</v>
       </c>
       <c r="B11" t="n">
-        <v>132911040898</v>
+        <v>134658223760</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911040898</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658223760</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -891,10 +891,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>334</v>
+        <v>377</v>
       </c>
       <c r="B12" t="n">
-        <v>132914194701</v>
+        <v>134634171809</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -923,7 +923,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914194701</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134634171809</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -934,10 +934,10 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>134</v>
+        <v>6567</v>
       </c>
       <c r="B13" t="n">
-        <v>132916788041</v>
+        <v>134628635768</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -949,11 +949,7 @@
           <t>Palmer</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>rocco_palmer160419466+106@infotech44.tech</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)2813 405223</t>
@@ -961,12 +957,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Boleyn  Grove, 7948</t>
+          <t>Sherwood  Vale, 7152</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916788041</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134628635768</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -977,10 +973,10 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>499</v>
+        <v>274</v>
       </c>
       <c r="B14" t="n">
-        <v>132916593529</v>
+        <v>134660791071</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -994,7 +990,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>rocco_palmer160419466+105@infotech44.tech</t>
+          <t>rocco_palmer160419466+106@infotech44.tech</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1004,12 +1000,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Buttonwood Walk, 9489</t>
+          <t>Boleyn  Grove, 7948</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916593529</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660791071</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1020,10 +1016,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>6935</v>
+        <v>634</v>
       </c>
       <c r="B15" t="n">
-        <v>132911173722</v>
+        <v>134632913267</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1035,7 +1031,11 @@
           <t>Palmer</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>rocco_palmer160419466+105@infotech44.tech</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)2813 405223</t>
@@ -1043,12 +1043,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Sherwood  Vale, 7152</t>
+          <t>Buttonwood Walk, 9489</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911173722</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134632913267</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1059,10 +1059,10 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>641</v>
+        <v>1047</v>
       </c>
       <c r="B16" t="n">
-        <v>132920811942</v>
+        <v>134654791805</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132920811942</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134654791805</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1102,10 +1102,10 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>42</v>
+        <v>153</v>
       </c>
       <c r="B17" t="n">
-        <v>132914893711</v>
+        <v>134627351992</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914893711</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134627351992</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1145,10 +1145,10 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1100</v>
+        <v>34</v>
       </c>
       <c r="B18" t="n">
-        <v>132912723045</v>
+        <v>134658223891</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912723045</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658223891</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1188,10 +1188,10 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>614</v>
+        <v>1072</v>
       </c>
       <c r="B19" t="n">
-        <v>132914893703</v>
+        <v>134654869508</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914893703</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134654869508</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1231,10 +1231,10 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>6803</v>
+        <v>5679</v>
       </c>
       <c r="B20" t="n">
-        <v>132922095119</v>
+        <v>134634171733</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922095119</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134634171733</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1270,10 +1270,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>501</v>
+        <v>643</v>
       </c>
       <c r="B21" t="n">
-        <v>132911703318</v>
+        <v>134632913266</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911703318</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134632913266</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1313,10 +1313,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>478</v>
+        <v>635</v>
       </c>
       <c r="B22" t="n">
-        <v>132913894432</v>
+        <v>134628635934</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132913894432</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134628635934</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1356,10 +1356,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>809</v>
+        <v>53</v>
       </c>
       <c r="B23" t="n">
-        <v>132922618789</v>
+        <v>134658954915</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922618789</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658954915</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1399,10 +1399,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>304</v>
+        <v>361</v>
       </c>
       <c r="B24" t="n">
-        <v>132924409170</v>
+        <v>134626150789</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>owen_wigley177952980@extex.org</t>
+          <t>owen_wigley177952980+102@extex.org</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1426,12 +1426,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Elystan  Drive, 8938</t>
+          <t>Kingly  Way, 4888</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924409170</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626150789</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1442,10 +1442,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>303</v>
+        <v>353</v>
       </c>
       <c r="B25" t="n">
-        <v>132912049799</v>
+        <v>134630045257</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>owen_wigley177952980+102@extex.org</t>
+          <t>owen_wigley177952980@extex.org</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1469,12 +1469,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Kingly  Way, 4888</t>
+          <t>Elystan  Drive, 8938</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912049799</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630045257</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1485,10 +1485,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>431</v>
+        <v>3815</v>
       </c>
       <c r="B26" t="n">
-        <v>132914154503</v>
+        <v>134659119514</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1500,11 +1500,7 @@
           <t>Tanner</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>noah_tanner17953585+102@acrit.org</t>
-        </is>
-      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)3156 686087</t>
@@ -1512,12 +1508,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Baylis  Alley, 9953</t>
+          <t>Canning  Way, 4293</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914154503</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134659119514</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1528,10 +1524,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1045</v>
+        <v>1061</v>
       </c>
       <c r="B27" t="n">
-        <v>132924535332</v>
+        <v>134656593521</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1545,7 +1541,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>noah_tanner17953585+101@acrit.org</t>
+          <t>noah_tanner17953585+103@acrit.org</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1555,12 +1551,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Clere  Avenue, 5521</t>
+          <t>Walnut Vale, 1387</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924535332</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134656593521</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1571,10 +1567,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>4111</v>
+        <v>165</v>
       </c>
       <c r="B28" t="n">
-        <v>132924273954</v>
+        <v>134625997062</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1586,7 +1582,11 @@
           <t>Tanner</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>noah_tanner17953585+102@acrit.org</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)3156 686087</t>
@@ -1594,12 +1594,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Canning  Way, 4293</t>
+          <t>Baylis  Alley, 9953</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924273954</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134625997062</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1610,10 +1610,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="B29" t="n">
-        <v>132914194705</v>
+        <v>134630081458</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>noah_tanner17953585+103@acrit.org</t>
+          <t>noah_tanner17953585+101@acrit.org</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1637,12 +1637,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Walnut Vale, 1387</t>
+          <t>Clere  Avenue, 5521</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914194705</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630081458</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1653,10 +1653,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>384</v>
+        <v>5587</v>
       </c>
       <c r="B30" t="n">
-        <v>132922688009</v>
+        <v>134660601760</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1668,11 +1668,7 @@
           <t>Roth</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>nate_roth902590743@liret.org</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)6807 838610</t>
@@ -1680,12 +1676,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Monroe Road, 4532</t>
+          <t>Thomas  Lane, 1184</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922688009</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660601760</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1696,10 +1692,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B31" t="n">
-        <v>132911795532</v>
+        <v>134626306083</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1713,7 +1709,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>nate_roth902590743+102@liret.org</t>
+          <t>nate_roth902590743@liret.org</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1723,12 +1719,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Maple Grove, 1863</t>
+          <t>Monroe Road, 4532</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911795532</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626306083</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1739,10 +1735,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>4910</v>
+        <v>36</v>
       </c>
       <c r="B32" t="n">
-        <v>132914339171</v>
+        <v>134633894246</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1754,7 +1750,11 @@
           <t>Roth</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>nate_roth902590743+106@liret.org</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)6807 838610</t>
@@ -1762,12 +1762,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Thomas  Lane, 1184</t>
+          <t>Thomas  Route, 9954</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914339171</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134633894246</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -1778,10 +1778,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1031</v>
+        <v>4714</v>
       </c>
       <c r="B33" t="n">
-        <v>132924535333</v>
+        <v>134660427924</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1793,11 +1793,7 @@
           <t>Roth</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>nate_roth902590743+106@liret.org</t>
-        </is>
-      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)6807 838610</t>
@@ -1805,12 +1801,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Thomas  Route, 9954</t>
+          <t>Carpenter Avenue, 4585</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924535333</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660427924</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1821,10 +1817,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>5625</v>
+        <v>1164</v>
       </c>
       <c r="B34" t="n">
-        <v>132922687857</v>
+        <v>134660466546</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1836,7 +1832,11 @@
           <t>Roth</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>nate_roth902590743+102@liret.org</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)6807 838610</t>
@@ -1844,12 +1844,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Carpenter Avenue, 4585</t>
+          <t>Maple Grove, 1863</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922687857</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660466546</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -1860,10 +1860,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>56</v>
+        <v>937</v>
       </c>
       <c r="B35" t="n">
-        <v>132924669846</v>
+        <v>134626230437</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924669846</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626230437</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1903,10 +1903,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>232</v>
+        <v>466</v>
       </c>
       <c r="B36" t="n">
-        <v>132924337835</v>
+        <v>134660284089</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>michael_veale472491137+102@gembat.biz</t>
+          <t>michael_veale472491137+103@gembat.biz</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1930,12 +1930,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Berriman  Lane, 9321</t>
+          <t>Bellenden   Drive, 6655</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924337835</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660284089</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -1946,10 +1946,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>318</v>
+        <v>1163</v>
       </c>
       <c r="B37" t="n">
-        <v>132914263144</v>
+        <v>134626385176</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>michael_veale472491137+103@gembat.biz</t>
+          <t>michael_veale472491137+102@gembat.biz</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1973,12 +1973,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Bellenden   Drive, 6655</t>
+          <t>Berriman  Lane, 9321</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914263144</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626385176</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -1989,10 +1989,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>1040</v>
+        <v>127</v>
       </c>
       <c r="B38" t="n">
-        <v>132916788030</v>
+        <v>134634171814</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916788030</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134634171814</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2032,10 +2032,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>5416</v>
+        <v>6720</v>
       </c>
       <c r="B39" t="n">
-        <v>132915331402</v>
+        <v>134632913179</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915331402</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134632913179</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2071,10 +2071,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>878</v>
+        <v>1055</v>
       </c>
       <c r="B40" t="n">
-        <v>132915056276</v>
+        <v>134658262369</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915056276</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658262369</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2114,10 +2114,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>5428</v>
+        <v>6531</v>
       </c>
       <c r="B41" t="n">
-        <v>132924473251</v>
+        <v>134654791715</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924473251</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134654791715</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2153,10 +2153,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>6397</v>
+        <v>6707</v>
       </c>
       <c r="B42" t="n">
-        <v>132922326611</v>
+        <v>134660238242</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922326611</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660238242</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2192,10 +2192,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>5250</v>
+        <v>4078</v>
       </c>
       <c r="B43" t="n">
-        <v>132915056210</v>
+        <v>134628635807</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2220,7 +2220,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915056210</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134628635807</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2231,10 +2231,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>1026</v>
+        <v>7</v>
       </c>
       <c r="B44" t="n">
-        <v>132912405820</v>
+        <v>134660466573</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912405820</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660466573</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2274,10 +2274,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>831</v>
+        <v>1717</v>
       </c>
       <c r="B45" t="n">
-        <v>132924732743</v>
+        <v>134658430878</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>leroy_dwyer505528803+101@brety.org</t>
+          <t>leroy_dwyer505528803@brety.org</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2301,12 +2301,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Emily  Way, 7361</t>
+          <t>Cavell   Street, 7744</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924732743</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658430878</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2317,10 +2317,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>1</v>
+        <v>1048</v>
       </c>
       <c r="B46" t="n">
-        <v>132898965405</v>
+        <v>134630655844</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>leroy_dwyer505528803@brety.org</t>
+          <t>leroy_dwyer505528803+101@brety.org</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2344,12 +2344,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Cavell   Street, 7744</t>
+          <t>Emily  Way, 7361</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132898965405</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630655844</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2360,10 +2360,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>124</v>
+        <v>5323</v>
       </c>
       <c r="B47" t="n">
-        <v>132923723037</v>
+        <v>134630293284</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2375,11 +2375,7 @@
           <t>Corbett</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>julius_corbett117840293+104@jiman.org</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)3628 508743</t>
@@ -2387,12 +2383,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>West Walk, 6366</t>
+          <t>Black Swan  Tunnel, 5780</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132923723037</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630293284</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2403,10 +2399,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>6547</v>
+        <v>159</v>
       </c>
       <c r="B48" t="n">
-        <v>132912343439</v>
+        <v>134630149520</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2418,7 +2414,11 @@
           <t>Corbett</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>julius_corbett117840293+104@jiman.org</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)3628 508743</t>
@@ -2426,12 +2426,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Black Swan  Tunnel, 5780</t>
+          <t>West Walk, 6366</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912343439</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630149520</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2442,10 +2442,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1006</v>
+        <v>232</v>
       </c>
       <c r="B49" t="n">
-        <v>132922754165</v>
+        <v>134626108968</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>julian_farrow1141858439+105@gembat.biz</t>
+          <t>julian_farrow1141858439@gembat.biz</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2469,12 +2469,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Cavaye  Rue, 6315</t>
+          <t>Andrews  Alley, 1970</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922754165</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626108968</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -2485,10 +2485,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B50" t="n">
-        <v>132923444149</v>
+        <v>134658188421</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2502,7 +2502,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>julian_farrow1141858439@gembat.biz</t>
+          <t>julian_farrow1141858439+105@gembat.biz</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2512,12 +2512,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Andrews  Alley, 1970</t>
+          <t>Cavaye  Rue, 6315</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132923444149</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658188421</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -2528,10 +2528,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>855</v>
+        <v>120</v>
       </c>
       <c r="B51" t="n">
-        <v>132924535335</v>
+        <v>134626150794</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924535335</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626150794</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -2571,10 +2571,10 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>5227</v>
+        <v>5663</v>
       </c>
       <c r="B52" t="n">
-        <v>132910294832</v>
+        <v>134657850389</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910294832</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134657850389</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -2610,10 +2610,10 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>60</v>
+        <v>992</v>
       </c>
       <c r="B53" t="n">
-        <v>132921138295</v>
+        <v>134660428044</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132921138295</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660428044</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -2653,10 +2653,10 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>851</v>
+        <v>1006</v>
       </c>
       <c r="B54" t="n">
-        <v>132915056278</v>
+        <v>134660466548</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915056278</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660466548</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -2696,10 +2696,10 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>3920</v>
+        <v>3914</v>
       </c>
       <c r="B55" t="n">
-        <v>132915666040</v>
+        <v>134627981934</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915666040</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134627981934</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -2735,10 +2735,10 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>5701</v>
+        <v>1019</v>
       </c>
       <c r="B56" t="n">
-        <v>132919827098</v>
+        <v>134656593522</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2750,7 +2750,11 @@
           <t>Nobbs</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>jack_nobbs214667606+104@supunk.biz</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)1043 56031</t>
@@ -2758,12 +2762,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Carol   Way, 7139</t>
+          <t>Sherlock   Alley, 7670</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919827098</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134656593522</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -2774,10 +2778,10 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>16</v>
+        <v>4965</v>
       </c>
       <c r="B57" t="n">
-        <v>132924473407</v>
+        <v>134631191607</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -2789,11 +2793,7 @@
           <t>Nobbs</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>jack_nobbs214667606+104@supunk.biz</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)1043 56031</t>
@@ -2801,12 +2801,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Sherlock   Alley, 7670</t>
+          <t>Carol   Way, 7139</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924473407</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134631191607</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -2817,10 +2817,10 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>4946</v>
+        <v>986</v>
       </c>
       <c r="B58" t="n">
-        <v>132924337759</v>
+        <v>134627220482</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2832,7 +2832,11 @@
           <t>Nobbs</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>jack_nobbs214667606@supunk.biz</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)1043 56031</t>
@@ -2840,12 +2844,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>College  Vale, 2300</t>
+          <t>Union  Pass, 9912</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924337759</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134627220482</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -2856,10 +2860,10 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>599</v>
+        <v>4451</v>
       </c>
       <c r="B59" t="n">
-        <v>132914460936</v>
+        <v>134631878264</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2871,11 +2875,7 @@
           <t>Nobbs</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>jack_nobbs214667606@supunk.biz</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)1043 56031</t>
@@ -2883,12 +2883,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Union  Pass, 9912</t>
+          <t>College  Vale, 2300</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914460936</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134631878264</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -2899,10 +2899,10 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>6667</v>
+        <v>5686</v>
       </c>
       <c r="B60" t="n">
-        <v>132919389523</v>
+        <v>134658954843</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919389523</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658954843</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -2938,10 +2938,10 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>4156</v>
+        <v>1024</v>
       </c>
       <c r="B61" t="n">
-        <v>132923081225</v>
+        <v>134634171802</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2953,7 +2953,11 @@
           <t>Tutton</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>harry_tutton509901574@typill.biz</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)7425 2015</t>
@@ -2961,12 +2965,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Camera  Vale, 8388</t>
+          <t>Thorndike   Route, 5913</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132923081225</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134634171802</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -2977,10 +2981,10 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>461</v>
+        <v>3798</v>
       </c>
       <c r="B62" t="n">
-        <v>132912771203</v>
+        <v>134654869405</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2992,11 +2996,7 @@
           <t>Tutton</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>harry_tutton509901574@typill.biz</t>
-        </is>
-      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)7425 2015</t>
@@ -3004,12 +3004,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Thorndike   Route, 5913</t>
+          <t>Camera  Vale, 8388</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912771203</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134654869405</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3020,10 +3020,10 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>446</v>
+        <v>155</v>
       </c>
       <c r="B63" t="n">
-        <v>132919389610</v>
+        <v>134626306084</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>hank_roberts1808907109+103@twipet.com</t>
+          <t>hank_roberts1808907109+104@twipet.com</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3047,12 +3047,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Canon Walk, 1444</t>
+          <t>Sheringham   Route, 2097</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919389610</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626306084</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -3063,10 +3063,10 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>194</v>
+        <v>602</v>
       </c>
       <c r="B64" t="n">
-        <v>132924473403</v>
+        <v>134633475843</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>hank_roberts1808907109+104@twipet.com</t>
+          <t>hank_roberts1808907109+103@twipet.com</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3090,12 +3090,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Sheringham   Route, 2097</t>
+          <t>Canon Walk, 1444</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924473403</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134633475843</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3106,10 +3106,10 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>986</v>
+        <v>1703</v>
       </c>
       <c r="B65" t="n">
-        <v>132914762347</v>
+        <v>134658223793</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>george_radcliffe235655210@nanoff.biz</t>
+          <t>george_radcliffe235655210+105@nanoff.biz</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3133,12 +3133,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Elf  Grove, 736</t>
+          <t>Ellerman   Hill, 5767</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914762347</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658223793</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -3149,10 +3149,10 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B66" t="n">
-        <v>132916927321</v>
+        <v>134657625728</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>george_radcliffe235655210+105@nanoff.biz</t>
+          <t>george_radcliffe235655210@nanoff.biz</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3176,12 +3176,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Ellerman   Hill, 5767</t>
+          <t>Elf  Grove, 736</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916927321</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134657625728</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -3192,10 +3192,10 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>53</v>
+        <v>1030</v>
       </c>
       <c r="B67" t="n">
-        <v>132914700648</v>
+        <v>134626787671</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>ethan_reynolds1948188016+103@fuliss.net</t>
+          <t>ethan_reynolds1948188016+102@fuliss.net</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3219,12 +3219,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Mariner  Road, 5893</t>
+          <t>Chamberlain  Walk, 1884</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914700648</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626787671</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -3235,10 +3235,10 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>569</v>
+        <v>944</v>
       </c>
       <c r="B68" t="n">
-        <v>132910630480</v>
+        <v>134660466549</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>ethan_reynolds1948188016+102@fuliss.net</t>
+          <t>ethan_reynolds1948188016+103@fuliss.net</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3262,12 +3262,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Chamberlain  Walk, 1884</t>
+          <t>Mariner  Road, 5893</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910630480</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660466549</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -3278,10 +3278,10 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>413</v>
+        <v>987</v>
       </c>
       <c r="B69" t="n">
-        <v>132919389609</v>
+        <v>134626230434</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>erick_holt2014841980+104@ovock.tech</t>
+          <t>erick_holt2014841980+102@ovock.tech</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3305,12 +3305,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Birkbeck  Route, 2358</t>
+          <t>Camera  Tunnel, 3496</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919389609</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626230434</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -3321,10 +3321,10 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>55</v>
+        <v>591</v>
       </c>
       <c r="B70" t="n">
-        <v>132912723060</v>
+        <v>134632497515</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>erick_holt2014841980+105@ovock.tech</t>
+          <t>erick_holt2014841980@ovock.tech</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3348,12 +3348,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Belgrave  Crossroad, 7401</t>
+          <t>Bales  Drive, 1780</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912723060</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134632497515</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -3364,10 +3364,10 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>204</v>
+        <v>941</v>
       </c>
       <c r="B71" t="n">
-        <v>132910757693</v>
+        <v>134630293349</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>erick_holt2014841980+102@ovock.tech</t>
+          <t>erick_holt2014841980+105@ovock.tech</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3391,12 +3391,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Camera  Tunnel, 3496</t>
+          <t>Belgrave  Crossroad, 7401</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910757693</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630293349</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -3407,10 +3407,10 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>436</v>
+        <v>589</v>
       </c>
       <c r="B72" t="n">
-        <v>132924535337</v>
+        <v>134626108962</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>erick_holt2014841980@ovock.tech</t>
+          <t>erick_holt2014841980+104@ovock.tech</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3434,12 +3434,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Bales  Drive, 1780</t>
+          <t>Birkbeck  Route, 2358</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924535337</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626108962</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -3450,10 +3450,10 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>48</v>
+        <v>5675</v>
       </c>
       <c r="B73" t="n">
-        <v>132919827230</v>
+        <v>134660790932</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -3465,11 +3465,7 @@
           <t>Long</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>eduardo_long1683975626+101@bretoux.com</t>
-        </is>
-      </c>
+      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)5850 843832</t>
@@ -3477,12 +3473,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Bacon  Lane, 3421</t>
+          <t>Birkenhead   Route, 5172</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919827230</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660790932</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -3493,10 +3489,10 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>6411</v>
+        <v>5513</v>
       </c>
       <c r="B74" t="n">
-        <v>132924273849</v>
+        <v>134626230378</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -3521,7 +3517,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924273849</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626230378</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -3532,10 +3528,10 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>5925</v>
+        <v>945</v>
       </c>
       <c r="B75" t="n">
-        <v>132922754092</v>
+        <v>134658430890</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -3547,7 +3543,11 @@
           <t>Long</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>eduardo_long1683975626+101@bretoux.com</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)5850 843832</t>
@@ -3555,12 +3555,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Birkenhead   Route, 5172</t>
+          <t>Bacon  Lane, 3421</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922754092</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658430890</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -3571,10 +3571,10 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>5957</v>
+        <v>6176</v>
       </c>
       <c r="B76" t="n">
-        <v>132912049729</v>
+        <v>134660427903</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912049729</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660427903</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -3610,10 +3610,10 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>196</v>
+        <v>1053</v>
       </c>
       <c r="B77" t="n">
-        <v>132922326683</v>
+        <v>134659072260</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922326683</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134659072260</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -3653,10 +3653,10 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>4949</v>
+        <v>158</v>
       </c>
       <c r="B78" t="n">
-        <v>132911703172</v>
+        <v>134626631529</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3668,7 +3668,11 @@
           <t>Boyle</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>denis_boyle1570473023@gompie.com</t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)6678 565525</t>
@@ -3676,12 +3680,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Chatfield  Crossroad, 5500</t>
+          <t>Clarks  Alley, 4115</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911703172</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626631529</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -3692,10 +3696,10 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>300</v>
+        <v>5529</v>
       </c>
       <c r="B79" t="n">
-        <v>132923159613</v>
+        <v>134633894163</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -3707,11 +3711,7 @@
           <t>Boyle</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>denis_boyle1570473023@gompie.com</t>
-        </is>
-      </c>
+      <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)6678 565525</t>
@@ -3719,12 +3719,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Clarks  Alley, 4115</t>
+          <t>Chatfield  Crossroad, 5500</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132923159613</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134633894163</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -3735,10 +3735,10 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>518</v>
+        <v>824</v>
       </c>
       <c r="B80" t="n">
-        <v>132915120462</v>
+        <v>134658223874</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915120462</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658223874</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -3778,10 +3778,10 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>107</v>
+        <v>248</v>
       </c>
       <c r="B81" t="n">
-        <v>132919389612</v>
+        <v>134658223884</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919389612</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658223884</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -3821,10 +3821,10 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>6784</v>
+        <v>6440</v>
       </c>
       <c r="B82" t="n">
-        <v>132924273840</v>
+        <v>134627262861</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924273840</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134627262861</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -3860,10 +3860,10 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>5834</v>
+        <v>976</v>
       </c>
       <c r="B83" t="n">
-        <v>132922618728</v>
+        <v>134626787672</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -3875,7 +3875,11 @@
           <t>Yard</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>clint_yard287681084+103@iatim.tech</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)7204 236315</t>
@@ -3883,12 +3887,12 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Chart   Avenue, 7832</t>
+          <t>Waldram Park  Grove, 6478</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922618728</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626787672</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -3899,10 +3903,10 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>567</v>
+        <v>139</v>
       </c>
       <c r="B84" t="n">
-        <v>132911299719</v>
+        <v>134659072273</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -3916,7 +3920,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>clint_yard287681084@iatim.tech</t>
+          <t>clint_yard287681084+102@iatim.tech</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3926,12 +3930,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Chambers  Street, 97</t>
+          <t>Coal Wharf  Pass, 6986</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911299719</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134659072273</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -3942,10 +3946,10 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>929</v>
+        <v>1005</v>
       </c>
       <c r="B85" t="n">
-        <v>132912049793</v>
+        <v>134626631518</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -3959,7 +3963,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>clint_yard287681084+102@iatim.tech</t>
+          <t>clint_yard287681084@iatim.tech</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3969,12 +3973,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Coal Wharf  Pass, 6986</t>
+          <t>Chambers  Street, 97</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912049793</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626631518</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -3985,10 +3989,10 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>198</v>
+        <v>4958</v>
       </c>
       <c r="B86" t="n">
-        <v>132916656031</v>
+        <v>134660841229</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -4000,11 +4004,7 @@
           <t>Yard</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>clint_yard287681084+103@iatim.tech</t>
-        </is>
-      </c>
+      <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)7204 236315</t>
@@ -4012,12 +4012,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Waldram Park  Grove, 6478</t>
+          <t>Chart   Avenue, 7832</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916656031</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660841229</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -4028,10 +4028,10 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>359</v>
+        <v>170</v>
       </c>
       <c r="B87" t="n">
-        <v>132912771204</v>
+        <v>134660357516</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -4060,7 +4060,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912771204</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660357516</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -4071,10 +4071,10 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>884</v>
+        <v>2</v>
       </c>
       <c r="B88" t="n">
-        <v>132914963046</v>
+        <v>134626787689</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914963046</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626787689</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -4114,10 +4114,10 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>193</v>
+        <v>979</v>
       </c>
       <c r="B89" t="n">
-        <v>132912771207</v>
+        <v>134660841278</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132912771207</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660841278</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -4157,10 +4157,10 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>184</v>
+        <v>75</v>
       </c>
       <c r="B90" t="n">
-        <v>132910294896</v>
+        <v>134657273268</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910294896</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134657273268</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -4200,10 +4200,10 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>5142</v>
+        <v>5107</v>
       </c>
       <c r="B91" t="n">
-        <v>132923231048</v>
+        <v>134626108833</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132923231048</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626108833</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -4239,10 +4239,10 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>4721</v>
+        <v>747</v>
       </c>
       <c r="B92" t="n">
-        <v>132910908081</v>
+        <v>134658466704</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -4254,7 +4254,11 @@
           <t>James</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>bryon_james964377164+101@gompie.com</t>
+        </is>
+      </c>
       <c r="F92" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)4240 711356</t>
@@ -4262,12 +4266,12 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Belmont Park Pass, 9584</t>
+          <t>Walnut Boulevard, 3808</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910908081</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658466704</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
@@ -4278,10 +4282,10 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>10</v>
+        <v>1602</v>
       </c>
       <c r="B93" t="n">
-        <v>132916788045</v>
+        <v>134610766009</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -4310,7 +4314,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916788045</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134610766009</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -4321,10 +4325,10 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>39</v>
+        <v>5660</v>
       </c>
       <c r="B94" t="n">
-        <v>132911498152</v>
+        <v>134629720582</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -4336,11 +4340,7 @@
           <t>James</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>bryon_james964377164+101@gompie.com</t>
-        </is>
-      </c>
+      <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)4240 711356</t>
@@ -4348,12 +4348,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Walnut Boulevard, 3808</t>
+          <t>Belmont Park Pass, 9584</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911498152</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134629720582</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -4364,10 +4364,10 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>311</v>
+        <v>174</v>
       </c>
       <c r="B95" t="n">
-        <v>132911703320</v>
+        <v>134659261966</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911703320</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134659261966</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -4407,10 +4407,10 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>0</v>
+        <v>3843</v>
       </c>
       <c r="B96" t="n">
-        <v>132923444151</v>
+        <v>134657273227</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -4422,11 +4422,7 @@
           <t>Turner</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>brad_turner714061428+101@bretoux.com</t>
-        </is>
-      </c>
+      <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)7012 324125</t>
@@ -4434,12 +4430,12 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Dyott   Alley, 6300</t>
+          <t>South Crossroad, 17</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132923444151</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134657273227</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -4450,10 +4446,10 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>5123</v>
+        <v>435</v>
       </c>
       <c r="B97" t="n">
-        <v>132914068356</v>
+        <v>134633702762</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -4465,7 +4461,11 @@
           <t>Turner</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>brad_turner714061428+101@bretoux.com</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)7012 324125</t>
@@ -4473,12 +4473,12 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>South Crossroad, 17</t>
+          <t>Dyott   Alley, 6300</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914068356</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134633702762</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -4489,10 +4489,10 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>4948</v>
+        <v>134</v>
       </c>
       <c r="B98" t="n">
-        <v>132914962985</v>
+        <v>134657273267</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -4504,7 +4504,11 @@
           <t>Nash</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>brad_nash201967772+104@ovock.tech</t>
+        </is>
+      </c>
       <c r="F98" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)2737 182784</t>
@@ -4512,12 +4516,12 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Blanchard  Pass, 3330</t>
+          <t>St. Johs  Tunnel, 1339</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914962985</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134657273267</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -4528,10 +4532,10 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="B99" t="n">
-        <v>132914700646</v>
+        <v>134660428054</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -4560,7 +4564,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914700646</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660428054</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -4571,10 +4575,10 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>923</v>
+        <v>6437</v>
       </c>
       <c r="B100" t="n">
-        <v>132924732741</v>
+        <v>134658430810</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -4586,11 +4590,7 @@
           <t>Nash</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>brad_nash201967772+104@ovock.tech</t>
-        </is>
-      </c>
+      <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(44)2737 182784</t>
@@ -4598,12 +4598,12 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>St. Johs  Tunnel, 1339</t>
+          <t>Blanchard  Pass, 3330</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924732741</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134658430810</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -4614,10 +4614,10 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>192</v>
+        <v>969</v>
       </c>
       <c r="B101" t="n">
-        <v>132910630489</v>
+        <v>134660357495</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -4646,7 +4646,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910630489</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660357495</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -4657,10 +4657,10 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>332</v>
+        <v>160</v>
       </c>
       <c r="B102" t="n">
-        <v>132924337833</v>
+        <v>134626230450</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924337833</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626230450</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -4700,10 +4700,10 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>410</v>
+        <v>564</v>
       </c>
       <c r="B103" t="n">
-        <v>132898965397</v>
+        <v>134654869516</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -4732,7 +4732,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132898965397</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134654869516</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -4743,10 +4743,10 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>43</v>
+        <v>914</v>
       </c>
       <c r="B104" t="n">
-        <v>132924732749</v>
+        <v>134630045247</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132924732749</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630045247</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
@@ -4786,10 +4786,10 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>2997</v>
+        <v>4066</v>
       </c>
       <c r="B105" t="n">
-        <v>132919827127</v>
+        <v>134660790962</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132919827127</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660790962</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -4825,10 +4825,10 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>249</v>
+        <v>1611</v>
       </c>
       <c r="B106" t="n">
-        <v>132915331473</v>
+        <v>134632913257</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -4842,7 +4842,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>barry_ryan1600445419+103@twace.org</t>
+          <t>barry_ryan1600445419+102@twace.org</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4852,12 +4852,12 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Boleyn  Drive, 2714</t>
+          <t>Chelsea Manor  Street, 3160</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915331473</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134632913257</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
@@ -4868,10 +4868,10 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>5122</v>
+        <v>5209</v>
       </c>
       <c r="B107" t="n">
-        <v>132914263087</v>
+        <v>134660790940</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -4896,7 +4896,7 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132914263087</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660790940</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
@@ -4907,10 +4907,10 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>20</v>
+        <v>395</v>
       </c>
       <c r="B108" t="n">
-        <v>132916788044</v>
+        <v>134631191666</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -4924,7 +4924,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>barry_ryan1600445419+102@twace.org</t>
+          <t>barry_ryan1600445419+103@twace.org</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4934,12 +4934,12 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Chelsea Manor  Street, 3160</t>
+          <t>Boleyn  Drive, 2714</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132916788044</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134631191666</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
@@ -4950,10 +4950,10 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>4769</v>
+        <v>6329</v>
       </c>
       <c r="B109" t="n">
-        <v>132910823864</v>
+        <v>134627262863</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910823864</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134627262863</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
@@ -4989,10 +4989,10 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>6620</v>
+        <v>6528</v>
       </c>
       <c r="B110" t="n">
-        <v>132911703138</v>
+        <v>134660566423</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -5012,12 +5012,12 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Baylis  Grove, 980</t>
+          <t>Chatsworth  Grove, 8137</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911703138</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134660566423</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -5028,10 +5028,10 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>6766</v>
+        <v>1578</v>
       </c>
       <c r="B111" t="n">
-        <v>132915666010</v>
+        <v>134633475758</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -5043,7 +5043,11 @@
           <t>Sinclair</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>anthony_sinclair1094808725+102@bungar.biz</t>
+        </is>
+      </c>
       <c r="F111" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)3505 033457</t>
@@ -5051,12 +5055,12 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Chatsworth  Grove, 8137</t>
+          <t>Arctic   Lane, 9179</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132915666010</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134633475758</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -5067,10 +5071,10 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>9</v>
+        <v>6701</v>
       </c>
       <c r="B112" t="n">
-        <v>132922326685</v>
+        <v>134628036517</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -5082,11 +5086,7 @@
           <t>Sinclair</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>anthony_sinclair1094808725+102@bungar.biz</t>
-        </is>
-      </c>
+      <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr">
         <is>
           <t xml:space="preserve"> +(353)3505 033457</t>
@@ -5094,12 +5094,12 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Arctic   Lane, 9179</t>
+          <t>Baylis  Grove, 980</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132922326685</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134628036517</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -5110,10 +5110,10 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>823</v>
+        <v>966</v>
       </c>
       <c r="B113" t="n">
-        <v>132911299715</v>
+        <v>134626631520</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>alan_warner22954315@fuliss.net</t>
+          <t>alan_warner22954315+101@fuliss.net</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -5137,12 +5137,12 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Bede  Avenue, 4773</t>
+          <t>Cedarne  Vale, 145</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132911299715</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134626631520</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -5153,10 +5153,10 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>524</v>
+        <v>1008</v>
       </c>
       <c r="B114" t="n">
-        <v>132910823976</v>
+        <v>134630809652</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -5170,7 +5170,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>alan_warner22954315+101@fuliss.net</t>
+          <t>alan_warner22954315@fuliss.net</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -5180,12 +5180,12 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Cedarne  Vale, 145</t>
+          <t>Bede  Avenue, 4773</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>https://app.hubspot.com/contacts/50189227/record/0-1/132910823976</t>
+          <t>https://app.hubspot.com/contacts/50189227/record/0-1/134630809652</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">

</xml_diff>